<commit_message>
Update download file ChromeDriver in cmd
</commit_message>
<xml_diff>
--- a/src/main/resources/data/dataTest.xlsx
+++ b/src/main/resources/data/dataTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ProjectEmployeeData\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BE10B4-157B-407E-907E-5290F4324875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A84427A-B842-401B-9136-FBA84E685A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-255" windowWidth="16440" windowHeight="28590" xr2:uid="{7F4866FA-B6DE-483E-A426-4081D2DD605E}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$G$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -504,7 +503,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,10 +613,10 @@
         <v>11</v>
       </c>
       <c r="H6" s="7">
-        <v>44867.333333333336</v>
+        <v>44866.333333333336</v>
       </c>
       <c r="I6" s="8">
-        <v>44867.708333333336</v>
+        <v>44866.708333333336</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -672,10 +671,10 @@
         <v>11</v>
       </c>
       <c r="H8" s="7">
-        <v>44867.333333333336</v>
+        <v>44866.333333333336</v>
       </c>
       <c r="I8" s="8">
-        <v>44867.708333333336</v>
+        <v>44866.708333333336</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>